<commit_message>
Commit Auto (Thu Jul  4 18:03:45     2024)
</commit_message>
<xml_diff>
--- a/INFO/Freezers_list_2_for_Metalgroup_(2).xlsx
+++ b/INFO/Freezers_list_2_for_Metalgroup_(2).xlsx
@@ -371,7 +371,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -405,12 +405,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -546,32 +540,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -847,7 +841,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -857,8 +851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -899,16 +893,16 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="29">
+      <c r="A4" s="27">
         <v>1</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="27" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="26" t="s">
         <v>26</v>
       </c>
       <c r="E4" s="10" t="s">
@@ -919,12 +913,12 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="31"/>
-      <c r="B5" s="31"/>
+      <c r="A5" s="28"/>
+      <c r="B5" s="28"/>
       <c r="C5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="25" t="s">
         <v>27</v>
       </c>
       <c r="E5" s="10" t="s">
@@ -964,7 +958,7 @@
       <c r="C7" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="26" t="s">
+      <c r="D7" s="25" t="s">
         <v>23</v>
       </c>
       <c r="E7" s="10" t="s">
@@ -975,16 +969,16 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A8" s="29">
+      <c r="A8" s="27">
         <v>4</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="27" t="s">
         <v>53</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" s="25" t="s">
         <v>56</v>
       </c>
       <c r="E8" s="10" t="s">
@@ -995,12 +989,12 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
-      <c r="B9" s="31"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="28"/>
       <c r="C9" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="25" t="s">
         <v>55</v>
       </c>
       <c r="E9" s="10" t="s">
@@ -1011,10 +1005,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="29">
+      <c r="A10" s="27">
         <v>5</v>
       </c>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="27" t="s">
         <v>48</v>
       </c>
       <c r="C10" s="13" t="s">
@@ -1031,8 +1025,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
-      <c r="B11" s="31"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="28"/>
       <c r="C11" s="13" t="s">
         <v>77</v>
       </c>
@@ -1076,13 +1070,13 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="33">
+      <c r="A18" s="29">
         <v>1</v>
       </c>
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="33" t="s">
+      <c r="C18" s="29" t="s">
         <v>22</v>
       </c>
       <c r="D18" s="6" t="s">
@@ -1096,9 +1090,9 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="33"/>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
+      <c r="A19" s="29"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
       <c r="D19" s="6" t="s">
         <v>29</v>
       </c>
@@ -1110,9 +1104,9 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="33"/>
-      <c r="B20" s="33"/>
-      <c r="C20" s="33"/>
+      <c r="A20" s="29"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
       <c r="D20" s="6" t="s">
         <v>18</v>
       </c>
@@ -1162,10 +1156,10 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="29">
+      <c r="A23" s="27">
         <v>4</v>
       </c>
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="27" t="s">
         <v>48</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -1182,8 +1176,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="31"/>
-      <c r="B24" s="31"/>
+      <c r="A24" s="28"/>
+      <c r="B24" s="28"/>
       <c r="C24" s="18" t="s">
         <v>81</v>
       </c>
@@ -1220,7 +1214,7 @@
       <c r="C29" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="11" t="s">
+      <c r="D29" s="33" t="s">
         <v>35</v>
       </c>
       <c r="E29" s="17" t="s">
@@ -1231,13 +1225,13 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="29">
+      <c r="A30" s="27">
         <v>2</v>
       </c>
-      <c r="B30" s="29" t="s">
+      <c r="B30" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="C30" s="29" t="s">
+      <c r="C30" s="27" t="s">
         <v>16</v>
       </c>
       <c r="D30" s="12" t="s">
@@ -1251,9 +1245,9 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="31"/>
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
+      <c r="A31" s="28"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="28"/>
       <c r="D31" s="12" t="s">
         <v>43</v>
       </c>
@@ -1285,16 +1279,16 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="29">
+      <c r="A33" s="27">
         <v>4</v>
       </c>
-      <c r="B33" s="29" t="s">
+      <c r="B33" s="27" t="s">
         <v>48</v>
       </c>
       <c r="C33" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="D33" s="28" t="s">
+      <c r="D33" s="30" t="s">
         <v>66</v>
       </c>
       <c r="E33" s="10" t="s">
@@ -1305,32 +1299,32 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="30"/>
-      <c r="B34" s="30"/>
+      <c r="A34" s="31"/>
+      <c r="B34" s="31"/>
       <c r="C34" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="D34" s="28"/>
+      <c r="D34" s="30"/>
       <c r="E34" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="F34" s="30"/>
+      <c r="F34" s="31"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="30"/>
-      <c r="B35" s="30"/>
+      <c r="A35" s="31"/>
+      <c r="B35" s="31"/>
       <c r="C35" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="D35" s="28"/>
+      <c r="D35" s="30"/>
       <c r="E35" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="F35" s="31"/>
+      <c r="F35" s="28"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="31"/>
-      <c r="B36" s="31"/>
+      <c r="A36" s="28"/>
+      <c r="B36" s="28"/>
       <c r="C36" s="13" t="s">
         <v>64</v>
       </c>
@@ -1363,13 +1357,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A8:A9"/>
     <mergeCell ref="D33:D35"/>
     <mergeCell ref="B33:B36"/>
     <mergeCell ref="A33:A36"/>
@@ -1381,6 +1368,13 @@
     <mergeCell ref="C30:C31"/>
     <mergeCell ref="B30:B31"/>
     <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A8:A9"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Commit Auto (Fri Jul 26 17:48:29     2024)
</commit_message>
<xml_diff>
--- a/INFO/Freezers_list_2_for_Metalgroup_(2).xlsx
+++ b/INFO/Freezers_list_2_for_Metalgroup_(2).xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs\OpenServer 5.4.3\domains\TimeForEeexperiments\INFO\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11DB1654-E28A-4872-A83B-F024179A67D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7908" yWindow="1584" windowWidth="10632" windowHeight="10332" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7905" yWindow="1590" windowWidth="10635" windowHeight="10335"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="85">
   <si>
     <t>Морозильные шкафы</t>
   </si>
@@ -183,10 +177,6 @@
   </si>
   <si>
     <t xml:space="preserve">IC72 SL 1,3-1 9003	</t>
-  </si>
-  <si>
-    <t>I60 VL 0,8-
-I60 VL 1,2-1</t>
   </si>
   <si>
     <t>http://surl.li/qugda</t>
@@ -324,12 +314,20 @@
   <si>
     <t>http://surl.li/quykn</t>
   </si>
+  <si>
+    <t>freezers_showcases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+            'freezers',
+            'freezers_ice_cream',</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -355,14 +353,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF2C2C2C"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -377,7 +367,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -387,12 +377,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -478,9 +462,9 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -497,10 +481,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -510,22 +491,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
@@ -537,7 +512,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -546,14 +520,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -570,9 +547,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -847,38 +822,38 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.88671875" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="24"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D2" s="20"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -895,225 +870,228 @@
         <v>6</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="28">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="25">
         <v>1</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="25" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>7</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="30"/>
-      <c r="B5" s="30"/>
+    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
       <c r="C5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="9" t="s">
         <v>17</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="9" t="s">
         <v>24</v>
       </c>
       <c r="F7" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A8" s="25">
+        <v>4</v>
+      </c>
+      <c r="B8" s="25" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="28">
-        <v>4</v>
-      </c>
-      <c r="B8" s="28" t="s">
+      <c r="C8" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="13" t="s">
+    </row>
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="E8" s="10" t="s">
+      <c r="D9" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="F8" s="14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="30"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="D9" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="28">
+      <c r="F9" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="25">
         <v>5</v>
       </c>
-      <c r="B10" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="13" t="s">
+      <c r="B10" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="D10" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="E10" s="10" t="s">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="F10" s="18" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="30"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="13" t="s">
+      <c r="D11" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="E11" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D11" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="F11" s="18" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="8"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="8"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="8"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C17" s="7" t="s">
+      <c r="F11" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C17" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="32">
+      <c r="D17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="29">
         <v>1</v>
       </c>
-      <c r="B18" s="32" t="s">
+      <c r="B18" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="32" t="s">
+      <c r="C18" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="9" t="s">
         <v>19</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="32"/>
-      <c r="B19" s="32"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="6" t="s">
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="29"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="9" t="s">
         <v>20</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="32"/>
-      <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="6" t="s">
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="29"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="21" t="s">
         <v>18</v>
       </c>
       <c r="E20" s="3"/>
@@ -1121,7 +1099,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>2</v>
       </c>
@@ -1131,17 +1109,17 @@
       <c r="C21" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="9" t="s">
         <v>33</v>
       </c>
       <c r="F21" s="3">
         <v>-18</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>3</v>
       </c>
@@ -1151,66 +1129,69 @@
       <c r="C22" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="25" t="s">
+      <c r="D22" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="9" t="s">
         <v>34</v>
       </c>
       <c r="F22" s="3">
         <v>-18</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A23" s="28">
+    <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="25">
         <v>4</v>
       </c>
-      <c r="B23" s="28" t="s">
+      <c r="B23" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D23" s="25" t="s">
+      <c r="D23" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E23" s="10" t="s">
+    </row>
+    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="27"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="F23" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="30"/>
-      <c r="B24" s="30"/>
-      <c r="C24" s="18" t="s">
+      <c r="D24" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="E24" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="E24" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="F24" s="18" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="8"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C28" s="16" t="s">
+      <c r="F24" s="15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="7"/>
+    </row>
+    <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="C28" s="13" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D28" s="20" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>1</v>
       </c>
@@ -1220,51 +1201,49 @@
       <c r="C29" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="27" t="s">
+      <c r="D29" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="E29" s="17" t="s">
+      <c r="E29" s="14" t="s">
         <v>12</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A30" s="28">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="25">
         <v>2</v>
       </c>
-      <c r="B30" s="28" t="s">
+      <c r="B30" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C30" s="28" t="s">
+      <c r="C30" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="E30" s="17" t="s">
+      <c r="D30" s="23"/>
+      <c r="E30" s="14" t="s">
         <v>14</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="30"/>
-      <c r="B31" s="30"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="12" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="27"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="E31" s="17" t="s">
-        <v>45</v>
+      <c r="E31" s="14" t="s">
+        <v>44</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>3</v>
       </c>
@@ -1274,87 +1253,87 @@
       <c r="C32" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="D32" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="E32" s="17" t="s">
+      <c r="E32" s="14" t="s">
         <v>39</v>
       </c>
       <c r="F32" s="3">
         <v>-20</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="28">
+    <row r="33" spans="1:6" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="25">
         <v>4</v>
       </c>
-      <c r="B33" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="C33" s="18" t="s">
+      <c r="B33" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D33" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F33" s="28" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="26"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="D33" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="E33" s="10" t="s">
+      <c r="D34" s="24"/>
+      <c r="E34" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="F34" s="26"/>
+    </row>
+    <row r="35" spans="1:6" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="26"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D35" s="24"/>
+      <c r="E35" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="F35" s="27"/>
+    </row>
+    <row r="36" spans="1:6" ht="46.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="27"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D36" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E36" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="F33" s="31" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="29"/>
-      <c r="B34" s="29"/>
-      <c r="C34" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="D34" s="33"/>
-      <c r="E34" s="23" t="s">
+      <c r="F36" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="F34" s="29"/>
-    </row>
-    <row r="35" spans="1:6" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="29"/>
-      <c r="B35" s="29"/>
-      <c r="C35" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="D35" s="33"/>
-      <c r="E35" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="F35" s="30"/>
-    </row>
-    <row r="36" spans="1:6" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="30"/>
-      <c r="B36" s="30"/>
-      <c r="C36" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="D36" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="E36" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="F36" s="21" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C37" s="5"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
@@ -1382,26 +1361,26 @@
     <mergeCell ref="B30:B31"/>
     <mergeCell ref="A30:A31"/>
   </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="E5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="E29" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="E30" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="E6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="E18" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="E19" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="E7" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="E22" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="E32" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="E31" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E33" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="E36" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="E35" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="E34" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="E10" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="E24" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="E21" r:id="rId18" xr:uid="{02AC31A6-7076-4BC2-9495-36DD942EE501}"/>
+    <hyperlink ref="E4" r:id="rId1"/>
+    <hyperlink ref="E5" r:id="rId2"/>
+    <hyperlink ref="E29" r:id="rId3"/>
+    <hyperlink ref="E30" r:id="rId4"/>
+    <hyperlink ref="E6" r:id="rId5"/>
+    <hyperlink ref="E18" r:id="rId6"/>
+    <hyperlink ref="E19" r:id="rId7"/>
+    <hyperlink ref="E7" r:id="rId8"/>
+    <hyperlink ref="E22" r:id="rId9"/>
+    <hyperlink ref="E32" r:id="rId10"/>
+    <hyperlink ref="E31" r:id="rId11"/>
+    <hyperlink ref="E33" r:id="rId12"/>
+    <hyperlink ref="E36" r:id="rId13"/>
+    <hyperlink ref="E35" r:id="rId14"/>
+    <hyperlink ref="E34" r:id="rId15"/>
+    <hyperlink ref="E10" r:id="rId16"/>
+    <hyperlink ref="E24" r:id="rId17"/>
+    <hyperlink ref="E21" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId19"/>

</xml_diff>